<commit_message>
Some updates of letter recognition
</commit_message>
<xml_diff>
--- a/single_digit/Results/5vs8_CNN_GL.xlsx
+++ b/single_digit/Results/5vs8_CNN_GL.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Group_Learning\single_digit\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF87414-93FA-4DC6-BFF3-69377C4FCDF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD42D8D4-E273-4AA1-A4BF-AFFEEA8001B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A4D5629-DDC9-4A37-80E7-A4A435BAA222}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0A4D5629-DDC9-4A37-80E7-A4A435BAA222}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN" sheetId="1" r:id="rId1"/>
     <sheet name="CNN+GL" sheetId="2" r:id="rId2"/>
+    <sheet name="CNN+GL_MV" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
   <si>
     <t xml:space="preserve">window </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,6 +124,2491 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CNN+GL(MV)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]SVM!$D$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CNN+GL_MV'!$B$28:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26509999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16930000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-33D3-4C1B-BAED-19334D351B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CNN+GL(Adaptive)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]SVM!$D$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CNN+GL'!$B$28:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.41590000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0499999999999988E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9599999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24759999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-33D3-4C1B-BAED-19334D351B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="517260784"/>
+        <c:axId val="517260128"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CNN!$F$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CNN!$F$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.33179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33179999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-33D3-4C1B-BAED-19334D351B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="517260784"/>
+        <c:axId val="517260128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="517260784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Window size</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1400">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="517260128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="517260128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Test</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> error</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1400">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="517260784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CNN+GL(MV)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]SVM!$D$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CNN+GL_MV'!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA26-45AD-8A76-DCA40F8581C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CNN+GL(Adaptive)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]SVM!$D$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CNN+GL'!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.14999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DA26-45AD-8A76-DCA40F8581C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="517260784"/>
+        <c:axId val="517260128"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[2]CNN!$F$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CNN!$F$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.9999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9999999999999993E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DA26-45AD-8A76-DCA40F8581C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="517260784"/>
+        <c:axId val="517260128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="517260784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Window size</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1400">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="517260128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="517260128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> error</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1400">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="517260784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A96AEA95-AD18-4690-9F3A-374E0414CCE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="圖表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0A1AA38-5B35-4A07-A6F2-3343C0A07112}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="SVM"/>
+      <sheetName val="GL_MV"/>
+      <sheetName val="GL_adaptive"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="7">
+          <cell r="D7">
+            <v>5</v>
+          </cell>
+          <cell r="E7">
+            <v>10</v>
+          </cell>
+          <cell r="F7">
+            <v>15</v>
+          </cell>
+          <cell r="G7">
+            <v>20</v>
+          </cell>
+          <cell r="H7">
+            <v>25</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="13">
+          <cell r="B13">
+            <v>0.26</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="13">
+          <cell r="B13">
+            <v>0.05</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="CNN"/>
+      <sheetName val="CNN+GL"/>
+      <sheetName val="CNN+GL_MV"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="12">
+          <cell r="F12">
+            <v>5</v>
+          </cell>
+          <cell r="G12">
+            <v>10</v>
+          </cell>
+          <cell r="H12">
+            <v>15</v>
+          </cell>
+          <cell r="I12">
+            <v>20</v>
+          </cell>
+          <cell r="J12">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="F13">
+            <v>0.31029999999999996</v>
+          </cell>
+          <cell r="G13">
+            <v>0.31029999999999996</v>
+          </cell>
+          <cell r="H13">
+            <v>0.31029999999999996</v>
+          </cell>
+          <cell r="I13">
+            <v>0.31029999999999996</v>
+          </cell>
+          <cell r="J13">
+            <v>0.31029999999999996</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="F14">
+            <v>0</v>
+          </cell>
+          <cell r="G14">
+            <v>0</v>
+          </cell>
+          <cell r="H14">
+            <v>0</v>
+          </cell>
+          <cell r="I14">
+            <v>0</v>
+          </cell>
+          <cell r="J14">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="13">
+          <cell r="B13">
+            <v>0.55999999999999994</v>
+          </cell>
+          <cell r="C13">
+            <v>0.48</v>
+          </cell>
+          <cell r="D13">
+            <v>0.19</v>
+          </cell>
+          <cell r="E13">
+            <v>0</v>
+          </cell>
+          <cell r="F13">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>0.43590000000000001</v>
+          </cell>
+          <cell r="C28">
+            <v>0.44000000000000006</v>
+          </cell>
+          <cell r="D28">
+            <v>0.37820000000000004</v>
+          </cell>
+          <cell r="E28">
+            <v>0.1777</v>
+          </cell>
+          <cell r="F28">
+            <v>0.13350000000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="13">
+          <cell r="B13">
+            <v>0.5</v>
+          </cell>
+          <cell r="C13">
+            <v>0.5</v>
+          </cell>
+          <cell r="D13">
+            <v>0.45</v>
+          </cell>
+          <cell r="E13">
+            <v>0.1</v>
+          </cell>
+          <cell r="F13">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>0.5</v>
+          </cell>
+          <cell r="C28">
+            <v>0.5</v>
+          </cell>
+          <cell r="D28">
+            <v>0.47899999999999998</v>
+          </cell>
+          <cell r="E28">
+            <v>0.1759</v>
+          </cell>
+          <cell r="F28">
+            <v>0.13999999999999999</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,81 +2908,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82751D7-CEC9-4A47-9053-B670E3828681}">
-  <dimension ref="A2:B27"/>
+  <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:10">
       <c r="B3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:10">
       <c r="B4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:10">
       <c r="B5">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:10">
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:10">
       <c r="B7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:10">
       <c r="B8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:10">
       <c r="B9">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:10">
       <c r="B10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="F11">
+        <v>0.33179999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.33179999999999998</v>
+      </c>
+      <c r="H11">
+        <v>0.33179999999999998</v>
+      </c>
+      <c r="I11">
+        <v>0.33179999999999998</v>
+      </c>
+      <c r="J11">
+        <v>0.33179999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="F12">
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="G12">
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="H12">
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="I12">
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="J12">
+        <v>6.9999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13">
         <f>AVERAGE(B3:B12)</f>
         <v>6.9999999999999993E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:10">
       <c r="B16">
         <v>0.4</v>
       </c>
@@ -571,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06305DA-4BBB-4C2F-9010-8C6B7BDC7A27}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -607,10 +3142,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -624,10 +3159,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -641,7 +3176,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
         <v>0.3</v>
@@ -658,10 +3193,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -675,10 +3210,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="B7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -692,10 +3227,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="B8">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -709,7 +3244,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -726,7 +3261,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -743,13 +3278,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="B11">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C11">
         <v>0.2</v>
       </c>
       <c r="D11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -763,7 +3298,7 @@
         <v>0.2</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -781,15 +3316,15 @@
       </c>
       <c r="B13">
         <f>AVERAGE(B3:B12)</f>
-        <v>0.35000000000000003</v>
+        <v>0.14999999999999997</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:F13" si="0">AVERAGE(C3:C12)</f>
-        <v>0.10999999999999999</v>
+        <v>0.3000000000000001</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -832,172 +3367,172 @@
     </row>
     <row r="18" spans="1:6">
       <c r="B18">
-        <v>0.42099999999999999</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="C18">
-        <v>0.32400000000000001</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="D18">
-        <v>0.13800000000000001</v>
+        <v>0.112</v>
       </c>
       <c r="E18">
-        <v>0.113</v>
+        <v>0.115</v>
       </c>
       <c r="F18">
-        <v>0.19800000000000001</v>
+        <v>0.246</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="B19">
-        <v>0.40400000000000003</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="C19">
-        <v>0.315</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="D19">
-        <v>0.13700000000000001</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="E19">
-        <v>6.2E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="F19">
-        <v>0.223</v>
+        <v>0.26100000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20">
-        <v>0.42599999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="C20">
-        <v>0.38500000000000001</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="D20">
-        <v>9.2999999999999999E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="E20">
-        <v>0.121</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="F20">
-        <v>0.224</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21">
-        <v>0.42799999999999999</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="C21">
-        <v>0.222</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="D21">
-        <v>0.1</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E21">
-        <v>8.1000000000000003E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="F21">
-        <v>0.218</v>
+        <v>0.26200000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="B22">
-        <v>0.39700000000000002</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="C22">
-        <v>0.14899999999999999</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="D22">
-        <v>0.13100000000000001</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="E22">
-        <v>0.108</v>
+        <v>0.111</v>
       </c>
       <c r="F22">
-        <v>0.23699999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="B23">
-        <v>0.36</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="C23">
-        <v>0.13600000000000001</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="D23">
-        <v>7.9000000000000001E-2</v>
+        <v>0.115</v>
       </c>
       <c r="E23">
-        <v>0.16400000000000001</v>
+        <v>0.114</v>
       </c>
       <c r="F23">
-        <v>0.23799999999999999</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="B24">
-        <v>0.23300000000000001</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="C24">
-        <v>0.16</v>
+        <v>0.19700000000000001</v>
       </c>
       <c r="D24">
-        <v>0.121</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E24">
-        <v>7.0000000000000007E-2</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="F24">
-        <v>0.24399999999999999</v>
+        <v>0.32200000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="B25">
-        <v>0.57299999999999995</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="C25">
-        <v>0.26900000000000002</v>
+        <v>0.436</v>
       </c>
       <c r="D25">
-        <v>0.20799999999999999</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="E25">
-        <v>7.8E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F25">
-        <v>0.23100000000000001</v>
+        <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26">
-        <v>0.55300000000000005</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="C26">
-        <v>0.32300000000000001</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="D26">
-        <v>0.20599999999999999</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="E26">
-        <v>8.1000000000000003E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F26">
-        <v>0.23899999999999999</v>
+        <v>0.22900000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27">
-        <v>0.27200000000000002</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="C27">
-        <v>0.121</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="D27">
-        <v>0.151</v>
+        <v>6.3E-2</v>
       </c>
       <c r="E27">
-        <v>0.14899999999999999</v>
+        <v>0.123</v>
       </c>
       <c r="F27">
-        <v>0.22</v>
+        <v>0.28299999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1006,23 +3541,23 @@
       </c>
       <c r="B28">
         <f>AVERAGE(B18:B27)</f>
-        <v>0.40669999999999995</v>
+        <v>0.41590000000000005</v>
       </c>
       <c r="C28">
         <f t="shared" ref="C28:F28" si="1">AVERAGE(C18:C27)</f>
-        <v>0.2404</v>
+        <v>0.4163</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>0.13639999999999999</v>
+        <v>8.0499999999999988E-2</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>0.10269999999999999</v>
+        <v>9.9599999999999994E-2</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>0.22720000000000001</v>
+        <v>0.24759999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1031,27 +3566,516 @@
       </c>
       <c r="B29">
         <f>STDEVA(B18:B27)</f>
-        <v>0.1057712941523679</v>
+        <v>5.9274221490739895E-2</v>
       </c>
       <c r="C29">
         <f t="shared" ref="C29:F29" si="2">STDEVA(C18:C27)</f>
-        <v>9.5111863963790927E-2</v>
+        <v>0.12610934408943159</v>
       </c>
       <c r="D29">
         <f t="shared" si="2"/>
-        <v>4.3405580798377134E-2</v>
+        <v>2.3200814161959477E-2</v>
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
-        <v>3.4396543754020181E-2</v>
+        <v>2.4500340133693354E-2</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>1.3603921003397017E-2</v>
+        <v>3.7366651798986003E-2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A669EFFF-3957-4635-94B0-01F3A9B99E19}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>0.6</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>0.2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B3:B12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:F13" si="0">AVERAGE(C3:C12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="F18">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <v>0.111</v>
+      </c>
+      <c r="E19">
+        <v>0.21</v>
+      </c>
+      <c r="F19">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="F20">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>0.496</v>
+      </c>
+      <c r="E21">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.17399999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>0.161</v>
+      </c>
+      <c r="E22">
+        <v>0.23</v>
+      </c>
+      <c r="F22">
+        <v>0.186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="E23">
+        <v>0.158</v>
+      </c>
+      <c r="F23">
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <v>0.125</v>
+      </c>
+      <c r="E24">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F24">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25">
+        <v>0.5</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25">
+        <v>0.5</v>
+      </c>
+      <c r="E25">
+        <v>0.312</v>
+      </c>
+      <c r="F25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26">
+        <v>0.5</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="E26">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="F26">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E27">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="F27">
+        <v>0.157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <f>AVERAGE(B18:B27)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:F28" si="1">AVERAGE(C18:C27)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0.26509999999999995</v>
+      </c>
+      <c r="E28">
+        <f>AVERAGE(E18:E27)</f>
+        <v>0.25</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0.16930000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <f>STDEVA(B18:B27)</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:F29" si="2">STDEVA(C18:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>0.16720542920478268</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>8.72964298620892E-2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>1.629621632977013E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>